<commit_message>
Excel Data driven Test
</commit_message>
<xml_diff>
--- a/src/test/java/data/Login_data.xlsx
+++ b/src/test/java/data/Login_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -397,7 +397,7 @@
   <cols>
     <col min="1" max="1" customWidth="true" width="25.6328125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.73828125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.16015625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="20.6328125" collapsed="true"/>
   </cols>
   <sheetData>

</xml_diff>